<commit_message>
- Contrução de Tabelas do projeto Cardápio Digital; - Exclusão de Tudo referente a boleta; - Correções em Funcionalidade de upload massivo em módulo de Chamados (Controle de Demandas);
</commit_message>
<xml_diff>
--- a/Api Vivo Apps/FilesTemplates/Extract_Matricula_Model.xlsx
+++ b/Api Vivo Apps/FilesTemplates/Extract_Matricula_Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A0151191\repo\Api-Vivo-Apps\Api Vivo Apps\FilesTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E45E87-464B-42E6-92AF-A42D350A7186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FCD350C-8AD8-4D62-9F32-CB6BA2C0D76C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Tipo msg</t>
   </si>
@@ -31,9 +31,6 @@
     <t>Ação</t>
   </si>
   <si>
-    <t>Matrícula</t>
-  </si>
-  <si>
     <t>Subgrupo empregados</t>
   </si>
   <si>
@@ -167,6 +164,15 @@
   </si>
   <si>
     <t>Serviço executado apenas P/Tel</t>
+  </si>
+  <si>
+    <t>Id-Relacao</t>
+  </si>
+  <si>
+    <t>Id-Demanda</t>
+  </si>
+  <si>
+    <t>Matricula</t>
   </si>
 </sst>
 </file>
@@ -544,210 +550,216 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AW1"/>
+  <dimension ref="A1:AY1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="65" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="12" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="25" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="18" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="12" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="25" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="8" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="18" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="10" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="9" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="14" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="6" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="21" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="18" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="14" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="8" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="10" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="32" bestFit="1" customWidth="1"/>
-    <col min="42" max="43" width="9" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="22" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="13" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="9" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="6" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="12" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="18" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="6" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="14" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="10" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="32" bestFit="1" customWidth="1"/>
+    <col min="44" max="45" width="9" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="22" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="13" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="9" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="6" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="12" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" ht="62.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:51" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="Q1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="S1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="W1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="X1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="Y1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AA1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AB1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AC1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AF1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AH1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AI1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AK1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AL1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AN1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AP1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AR1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AT1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AV1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AW1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AX1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AY1" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="AW1" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>